<commit_message>
Fixed bug of a file handle and cleaned the code for debug at AWARESensor
</commit_message>
<xml_diff>
--- a/docs/AWARE-iOS-sensors.xlsx
+++ b/docs/AWARE-iOS-sensors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="33600" yWindow="-3380" windowWidth="25600" windowHeight="18520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Android Wear</t>
   </si>
   <si>
-    <t>△</t>
-  </si>
-  <si>
     <t>Applications</t>
   </si>
   <si>
@@ -183,6 +180,10 @@
   </si>
   <si>
     <t>Note</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>△</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -918,7 +919,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -939,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -957,7 +958,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -965,17 +966,17 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="16"/>
       <c r="F3" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="19" thickBot="1">
@@ -983,7 +984,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -993,12 +994,12 @@
         <v>5</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -1010,7 +1011,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -1022,7 +1023,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1034,7 +1035,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -1046,7 +1047,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
@@ -1058,7 +1059,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>5</v>
@@ -1070,10 +1071,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
@@ -1082,24 +1083,24 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>3</v>
@@ -1108,7 +1109,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -1120,7 +1121,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -1132,7 +1133,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -1144,7 +1145,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>5</v>
@@ -1156,21 +1157,21 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -1182,7 +1183,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
@@ -1194,7 +1195,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
@@ -1206,7 +1207,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>3</v>
@@ -1218,7 +1219,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>3</v>
@@ -1230,7 +1231,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>3</v>
@@ -1242,10 +1243,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
@@ -1254,10 +1255,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
@@ -1266,7 +1267,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
@@ -1278,10 +1279,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>
@@ -1290,7 +1291,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
@@ -1302,10 +1303,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
@@ -1314,7 +1315,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1326,7 +1327,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -1338,10 +1339,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>3</v>
@@ -1350,10 +1351,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>3</v>
@@ -1362,7 +1363,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>

</xml_diff>